<commit_message>
calorimetry : gui regression tests : NMR, spectrophotometry
</commit_message>
<xml_diff>
--- a/tests/data.gui/stable/spectrophotometry/dsl.3.no.ext/kev.constants.data.xlsx
+++ b/tests/data.gui/stable/spectrophotometry/dsl.3.no.ext/kev.constants.data.xlsx
@@ -254,16 +254,16 @@
     <t xml:space="preserve">OK</t>
   </si>
   <si>
-    <t xml:space="preserve">4.57094693183899</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.108730034369404</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.47013266563416</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.260060079433111</t>
+    <t xml:space="preserve">4.571025390625</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.108717276173831</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.46953125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.260200371728513</t>
   </si>
   <si>
     <t xml:space="preserve">Adj. R^2</t>
@@ -767,12 +767,12 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.848969562068136</v>
+        <v>0.848847310230273</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.848969562068136</v>
+        <v>0.848847310230273</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.999944167785635</v>
+        <v>0.999944167667562</v>
       </c>
     </row>
   </sheetData>
@@ -847,19 +847,19 @@
         <v>200</v>
       </c>
       <c r="C2" t="n">
-        <v>3.63384902787114</v>
+        <v>3.62851768723924</v>
       </c>
       <c r="D2" t="n">
-        <v>2964.50958508043</v>
+        <v>2964.36394125175</v>
       </c>
       <c r="E2" t="n">
-        <v>4768.81953495453</v>
+        <v>4768.81513735542</v>
       </c>
       <c r="F2" t="n">
-        <v>5054.57960446455</v>
+        <v>5055.18778225329</v>
       </c>
       <c r="G2" t="n">
-        <v>422942.732748066</v>
+        <v>423108.972180095</v>
       </c>
     </row>
     <row r="3">
@@ -870,19 +870,19 @@
         <v>300</v>
       </c>
       <c r="C3" t="n">
-        <v>22.5113678877864</v>
+        <v>22.5538789403126</v>
       </c>
       <c r="D3" t="n">
-        <v>8048.2325688426</v>
+        <v>8048.51242828701</v>
       </c>
       <c r="E3" t="n">
-        <v>6303.25890524787</v>
+        <v>6303.21573312717</v>
       </c>
       <c r="F3" t="n">
-        <v>3316.74562567488</v>
+        <v>3311.39032240926</v>
       </c>
       <c r="G3" t="n">
-        <v>-639021.551289459</v>
+        <v>-639364.45312061</v>
       </c>
     </row>
     <row r="4">
@@ -893,19 +893,19 @@
         <v>200</v>
       </c>
       <c r="C4" t="n">
-        <v>2.25385330039595</v>
+        <v>2.2557199599467</v>
       </c>
       <c r="D4" t="n">
-        <v>70.2021545853265</v>
+        <v>70.1880926029722</v>
       </c>
       <c r="E4" t="n">
-        <v>12.6708023024833</v>
+        <v>12.6654507470743</v>
       </c>
       <c r="F4" t="n">
-        <v>163.831291326674</v>
+        <v>164.100837409176</v>
       </c>
       <c r="G4" t="n">
-        <v>109243.711107637</v>
+        <v>109207.061021345</v>
       </c>
     </row>
     <row r="5">
@@ -916,19 +916,19 @@
         <v>300</v>
       </c>
       <c r="C5" t="n">
-        <v>1.8027054123765</v>
+        <v>1.80524215495195</v>
       </c>
       <c r="D5" t="n">
-        <v>56.1499739176578</v>
+        <v>56.1712028941527</v>
       </c>
       <c r="E5" t="n">
-        <v>10.1345211269192</v>
+        <v>10.1361011145313</v>
       </c>
       <c r="F5" t="n">
-        <v>131.037612580793</v>
+        <v>131.329134207315</v>
       </c>
       <c r="G5" t="n">
-        <v>87376.6847412983</v>
+        <v>87397.9011910678</v>
       </c>
     </row>
   </sheetData>
@@ -1326,138 +1326,138 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6.57167626841221e-08</v>
+        <v>0.0000000657079255915789</v>
       </c>
       <c r="B2" t="n">
-        <v>0.000353335405410957</v>
+        <v>0.000353335365591123</v>
       </c>
       <c r="C2" t="n">
-        <v>8.64590084348246e-07</v>
+        <v>0.000000864629911626739</v>
       </c>
       <c r="D2" t="n">
-        <v>4.50476505622661e-12</v>
+        <v>0.00000000000449732084461406</v>
       </c>
       <c r="E2" t="n">
-        <v>2.30315856505498e-07</v>
+        <v>0.000000230346831802918</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>8.4001348557892e-05</v>
+        <v>0.0000839967070662358</v>
       </c>
       <c r="B3" t="n">
-        <v>8.57882020990969e-05</v>
+        <v>0.0000857807350894835</v>
       </c>
       <c r="C3" t="n">
-        <v>0.000268324764177118</v>
+        <v>0.000268335056694733</v>
       </c>
       <c r="D3" t="n">
-        <v>1.78703372421423e-06</v>
+        <v>0.00000178420821621364</v>
       </c>
       <c r="E3" t="n">
-        <v>1.8018297020471e-10</v>
+        <v>0.000000000180192926758746</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.000347574362442624</v>
+        <v>0.000347583618662726</v>
       </c>
       <c r="B4" t="n">
-        <v>2.46740242897292e-05</v>
+        <v>0.000024670213965408</v>
       </c>
       <c r="C4" t="n">
-        <v>0.000319326274765001</v>
+        <v>0.000319343151640457</v>
       </c>
       <c r="D4" t="n">
-        <v>8.7997052027367e-06</v>
+        <v>0.00000878663865680689</v>
       </c>
       <c r="E4" t="n">
-        <v>4.35464007701678e-11</v>
+        <v>0.0000000000435452411209539</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.000665648939535394</v>
+        <v>0.000665672088035321</v>
       </c>
       <c r="B5" t="n">
-        <v>1.31508857689604e-05</v>
+        <v>0.0000131491284715596</v>
       </c>
       <c r="C5" t="n">
-        <v>0.00032594714525971</v>
+        <v>0.00032597380835523</v>
       </c>
       <c r="D5" t="n">
-        <v>1.72019689717009e-05</v>
+        <v>0.0000171770631735829</v>
       </c>
       <c r="E5" t="n">
-        <v>2.27381305450984e-11</v>
+        <v>0.0000000000227373398350435</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.0013330579651414</v>
+        <v>0.00133310373218991</v>
       </c>
       <c r="B6" t="n">
-        <v>6.36878430281812e-06</v>
+        <v>0.00000636835440170605</v>
       </c>
       <c r="C6" t="n">
-        <v>0.000316120388153839</v>
+        <v>0.000316167015005058</v>
       </c>
       <c r="D6" t="n">
-        <v>3.34108307598665e-05</v>
+        <v>0.0000333646338094201</v>
       </c>
       <c r="E6" t="n">
-        <v>1.13540542723186e-11</v>
+        <v>0.0000000000113536644740305</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.00264704835806024</v>
+        <v>0.00264712583306349</v>
       </c>
       <c r="B7" t="n">
-        <v>2.94394324161017e-06</v>
+        <v>0.00000294410784641187</v>
       </c>
       <c r="C7" t="n">
-        <v>0.000290160465876497</v>
+        <v>0.000290237611670279</v>
       </c>
       <c r="D7" t="n">
-        <v>6.08955909026936e-05</v>
+        <v>0.0000608182805040659</v>
       </c>
       <c r="E7" t="n">
-        <v>5.71792065614301e-12</v>
+        <v>0.00000000000571775330636466</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.00664385387229889</v>
+        <v>0.00664397774570443</v>
       </c>
       <c r="B8" t="n">
-        <v>9.35329944465505e-07</v>
+        <v>0.000000935641668413102</v>
       </c>
       <c r="C8" t="n">
-        <v>0.000231383210177002</v>
+        <v>0.000231506460134426</v>
       </c>
       <c r="D8" t="n">
-        <v>0.000121881459947133</v>
+        <v>0.000121757898265341</v>
       </c>
       <c r="E8" t="n">
-        <v>2.27813747491784e-12</v>
+        <v>0.00000000000227809500026514</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.0134042877665934</v>
+        <v>0.0134044254224832</v>
       </c>
       <c r="B9" t="n">
-        <v>3.43417561645228e-07</v>
+        <v>0.00000034362691489237</v>
       </c>
       <c r="C9" t="n">
-        <v>0.000171400930360845</v>
+        <v>0.00017153816754401</v>
       </c>
       <c r="D9" t="n">
-        <v>0.000182155652118493</v>
+        <v>0.000182018205581655</v>
       </c>
       <c r="E9" t="n">
-        <v>1.1291620075543e-12</v>
+        <v>0.00000000000112915041169726</v>
       </c>
     </row>
   </sheetData>
@@ -1514,28 +1514,28 @@
         <v>200</v>
       </c>
       <c r="C2" t="n">
-        <v>1.14899994949316</v>
+        <v>1.14899994954435</v>
       </c>
       <c r="D2" t="n">
-        <v>1.54332648404101</v>
+        <v>1.5433261305592</v>
       </c>
       <c r="E2" t="n">
-        <v>1.64171601946887</v>
+        <v>1.64171769433111</v>
       </c>
       <c r="F2" t="n">
-        <v>1.68274624679144</v>
+        <v>1.68274593717371</v>
       </c>
       <c r="G2" t="n">
-        <v>1.70012804176895</v>
+        <v>1.70012665074334</v>
       </c>
       <c r="H2" t="n">
-        <v>1.70987325013526</v>
+        <v>1.70987231378232</v>
       </c>
       <c r="I2" t="n">
-        <v>1.74640083440616</v>
+        <v>1.74640288825853</v>
       </c>
       <c r="J2" t="n">
-        <v>1.78782804934424</v>
+        <v>1.78782732674432</v>
       </c>
     </row>
     <row r="3">
@@ -1546,28 +1546,28 @@
         <v>300</v>
       </c>
       <c r="C3" t="n">
-        <v>2.7019999511069</v>
+        <v>2.70199995089303</v>
       </c>
       <c r="D3" t="n">
-        <v>2.3894668422014</v>
+        <v>2.38946851601394</v>
       </c>
       <c r="E3" t="n">
-        <v>2.24836140197627</v>
+        <v>2.24835480918796</v>
       </c>
       <c r="F3" t="n">
-        <v>2.23239532649969</v>
+        <v>2.23239307233761</v>
       </c>
       <c r="G3" t="n">
-        <v>2.18466303856759</v>
+        <v>2.18466740939406</v>
       </c>
       <c r="H3" t="n">
-        <v>2.11421029064477</v>
+        <v>2.11421833415463</v>
       </c>
       <c r="I3" t="n">
-        <v>2.01980661505828</v>
+        <v>2.01979962465506</v>
       </c>
       <c r="J3" t="n">
-        <v>1.98906043905376</v>
+        <v>1.9890621527603</v>
       </c>
     </row>
     <row r="4">
@@ -1578,28 +1578,28 @@
         <v>200</v>
       </c>
       <c r="C4" t="n">
-        <v>-5.05068364908823e-08</v>
+        <v>-0.0000000504556501024211</v>
       </c>
       <c r="D4" t="n">
-        <v>0.000326484041010655</v>
+        <v>0.000326130559196391</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.000283980531124994</v>
+        <v>-0.000282305668892313</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.00225375320855803</v>
+        <v>-0.00225406282629392</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.000871958231049019</v>
+        <v>-0.000873349256657052</v>
       </c>
       <c r="H4" t="n">
-        <v>0.00587325013525608</v>
+        <v>0.00587231378232156</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.00359916559384343</v>
+        <v>-0.00359711174146571</v>
       </c>
       <c r="J4" t="n">
-        <v>0.000828049344244297</v>
+        <v>0.000827326744315293</v>
       </c>
     </row>
     <row r="5">
@@ -1610,28 +1610,28 @@
         <v>300</v>
       </c>
       <c r="C5" t="n">
-        <v>-4.88930962383449e-08</v>
+        <v>-0.0000000491069669372735</v>
       </c>
       <c r="D5" t="n">
-        <v>0.000466842201398698</v>
+        <v>0.000468516013935272</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.00363859802372657</v>
+        <v>-0.00364519081203563</v>
       </c>
       <c r="F5" t="n">
-        <v>0.00439532649968877</v>
+        <v>0.00439307233761443</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.00133696143241169</v>
+        <v>-0.00133259060594426</v>
       </c>
       <c r="H5" t="n">
-        <v>0.000210290644774069</v>
+        <v>0.00021833415462913</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.000193384941721941</v>
+        <v>-0.000200375344935111</v>
       </c>
       <c r="J5" t="n">
-        <v>6.04390537617405e-05</v>
+        <v>0.0000621527603048566</v>
       </c>
     </row>
   </sheetData>
@@ -1688,28 +1688,28 @@
         <v>200</v>
       </c>
       <c r="C2" t="n">
-        <v>1.14899994949316</v>
+        <v>1.14899994954435</v>
       </c>
       <c r="D2" t="n">
-        <v>1.54332648404101</v>
+        <v>1.5433261305592</v>
       </c>
       <c r="E2" t="n">
-        <v>1.64171601946887</v>
+        <v>1.64171769433111</v>
       </c>
       <c r="F2" t="n">
-        <v>1.68274624679144</v>
+        <v>1.68274593717371</v>
       </c>
       <c r="G2" t="n">
-        <v>1.70012804176895</v>
+        <v>1.70012665074334</v>
       </c>
       <c r="H2" t="n">
-        <v>1.70987325013526</v>
+        <v>1.70987231378232</v>
       </c>
       <c r="I2" t="n">
-        <v>1.74640083440616</v>
+        <v>1.74640288825853</v>
       </c>
       <c r="J2" t="n">
-        <v>1.78782804934424</v>
+        <v>1.78782732674432</v>
       </c>
     </row>
     <row r="3">
@@ -1720,28 +1720,28 @@
         <v>300</v>
       </c>
       <c r="C3" t="n">
-        <v>2.7019999511069</v>
+        <v>2.70199995089303</v>
       </c>
       <c r="D3" t="n">
-        <v>2.3894668422014</v>
+        <v>2.38946851601394</v>
       </c>
       <c r="E3" t="n">
-        <v>2.24836140197627</v>
+        <v>2.24835480918796</v>
       </c>
       <c r="F3" t="n">
-        <v>2.23239532649969</v>
+        <v>2.23239307233761</v>
       </c>
       <c r="G3" t="n">
-        <v>2.18466303856759</v>
+        <v>2.18466740939406</v>
       </c>
       <c r="H3" t="n">
-        <v>2.11421029064477</v>
+        <v>2.11421833415463</v>
       </c>
       <c r="I3" t="n">
-        <v>2.01980661505828</v>
+        <v>2.01979962465506</v>
       </c>
       <c r="J3" t="n">
-        <v>1.98906043905376</v>
+        <v>1.9890621527603</v>
       </c>
     </row>
     <row r="4">
@@ -1752,28 +1752,28 @@
         <v>200</v>
       </c>
       <c r="C4" t="n">
-        <v>-4.39572119154763e-08</v>
+        <v>-0.000000043912663274518</v>
       </c>
       <c r="D4" t="n">
-        <v>0.000211590434874047</v>
+        <v>0.000211361347502522</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.000172947948309984</v>
+        <v>-0.000171927934769984</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.00133753899617687</v>
+        <v>-0.00133772274557503</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.000512615068223997</v>
+        <v>-0.000513432837540889</v>
       </c>
       <c r="H4" t="n">
-        <v>0.00344674303712211</v>
+        <v>0.00344619353422627</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.00205666605362482</v>
+        <v>-0.00205549242369469</v>
       </c>
       <c r="J4" t="n">
-        <v>0.000463374003494291</v>
+        <v>0.000462969638676717</v>
       </c>
     </row>
     <row r="5">
@@ -1784,28 +1784,28 @@
         <v>300</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.80951503472779e-08</v>
+        <v>-0.0000000181743030855934</v>
       </c>
       <c r="D5" t="n">
-        <v>0.000195413227877228</v>
+        <v>0.000196113861002625</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.00161571848300469</v>
+        <v>-0.00161864600889681</v>
       </c>
       <c r="F5" t="n">
-        <v>0.00197276772876516</v>
+        <v>0.00197175598636195</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.000611601753161797</v>
+        <v>-0.00060960229000195</v>
       </c>
       <c r="H5" t="n">
-        <v>9.94752340463904e-05</v>
+        <v>0.000103280110988235</v>
       </c>
       <c r="I5" t="n">
-        <v>-9.57351196643274e-05</v>
+        <v>-0.0000991957153144113</v>
       </c>
       <c r="J5" t="n">
-        <v>3.03866534749827e-05</v>
+        <v>0.0000312482455026931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>